<commit_message>
added skewed plot #2
</commit_message>
<xml_diff>
--- a/GAUSS_SKEWED/jump_freq_800/Simulation_Spectra_Avg/800Hz_simulation_15sigma_lognormal_skewed1.xlsx
+++ b/GAUSS_SKEWED/jump_freq_800/Simulation_Spectra_Avg/800Hz_simulation_15sigma_lognormal_skewed1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbhatia/Ninja/Sabyasachi_Sen/Files/GAUSS/jump_freq_800/Simulation_Spectra_Avg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbhatia/Ninja/Sabyasachi_Sen/Files/GAUSS_SKEWED/jump_freq_800/Simulation_Spectra_Avg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A801C1-A2F5-C744-8A9E-D4C67596A798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193A0F7F-A25D-8847-BE26-62D4BDA1DD75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="460" windowWidth="23040" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ppm</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Exponent of lognrmal dist</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>pdf * weight</t>
   </si>
 </sst>
 </file>
@@ -942,7 +948,7 @@
   <dimension ref="A1:O1367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1117,8 +1123,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
+      <c r="A4" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -1159,7 +1165,9 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B5" s="11">
         <f t="shared" ref="B5:F5" si="1">B3*B4</f>
         <v>2.6800390521772234E-4</v>
@@ -1206,7 +1214,9 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">

</xml_diff>